<commit_message>
Merging soils datas (begin analysis)
</commit_message>
<xml_diff>
--- a/Notebook/Data/soils/sols_CompletProfilCode.xlsx
+++ b/Notebook/Data/soils/sols_CompletProfilCode.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thsch\Desktop\Bachelor_Thesis_2017_Sources\Notebook\Data\soils\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="0" windowWidth="28800" windowHeight="13335"/>
+    <workbookView xWindow="4728" yWindow="0" windowWidth="28800" windowHeight="13332"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,9 +642,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,31 +928,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.44140625" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1051,7 +1054,7 @@
       <c r="M2">
         <v>5.9</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="5">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O2" t="s">
@@ -1073,7 +1076,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1113,7 +1116,7 @@
       <c r="M3">
         <v>6</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="5">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="O3" t="s">
@@ -1135,7 +1138,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1175,7 +1178,7 @@
       <c r="M4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <v>0.13600000000000001</v>
       </c>
       <c r="O4">
@@ -1197,7 +1200,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1237,7 +1240,7 @@
       <c r="M5">
         <v>5.4</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="5">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O5">
@@ -1259,7 +1262,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1299,7 +1302,7 @@
       <c r="M6">
         <v>5.5</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="5">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="O6">
@@ -1321,7 +1324,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1361,7 +1364,7 @@
       <c r="M7">
         <v>5.6</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O7">
@@ -1383,7 +1386,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1423,7 +1426,7 @@
       <c r="M8">
         <v>5.5</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="O8" t="s">
@@ -1445,7 +1448,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1485,7 +1488,7 @@
       <c r="M9">
         <v>5.4</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="O9" t="s">
@@ -1507,7 +1510,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1547,7 +1550,7 @@
       <c r="M10">
         <v>5.7</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="5">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="O10" t="s">
@@ -1569,7 +1572,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1609,7 +1612,7 @@
       <c r="M11" t="s">
         <v>107</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O11" t="s">
@@ -1631,7 +1634,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1671,7 +1674,7 @@
       <c r="M12">
         <v>5.8</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="5">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="O12">
@@ -1693,7 +1696,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1733,7 +1736,7 @@
       <c r="M13">
         <v>5.9</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O13">
@@ -1755,7 +1758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1795,7 +1798,7 @@
       <c r="M14">
         <v>5.0999999999999996</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O14" t="s">
@@ -1817,7 +1820,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1857,7 +1860,7 @@
       <c r="M15">
         <v>5.3</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O15" t="s">
@@ -1879,7 +1882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1919,7 +1922,7 @@
       <c r="M16">
         <v>5.0999999999999996</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O16" t="s">
@@ -1941,7 +1944,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1981,7 +1984,7 @@
       <c r="M17">
         <v>5.2</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="5">
         <v>5.5E-2</v>
       </c>
       <c r="O17" t="s">
@@ -2003,7 +2006,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2043,7 +2046,7 @@
       <c r="M18">
         <v>5.8</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="5">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="O18" t="s">
@@ -2065,7 +2068,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2105,7 +2108,7 @@
       <c r="M19">
         <v>5.5</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="5">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O19" t="s">
@@ -2127,7 +2130,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2167,7 +2170,7 @@
       <c r="M20">
         <v>5.7</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="5">
         <v>3.1E-2</v>
       </c>
       <c r="O20" t="s">
@@ -2189,7 +2192,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2229,7 +2232,7 @@
       <c r="M21">
         <v>6</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="5">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="O21" t="s">
@@ -2251,7 +2254,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2291,7 +2294,7 @@
       <c r="M22" t="s">
         <v>107</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O22" t="s">
@@ -2313,7 +2316,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2353,7 +2356,7 @@
       <c r="M23">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="O23">
@@ -2375,7 +2378,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2415,7 +2418,7 @@
       <c r="M24">
         <v>5.0999999999999996</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="5">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="O24">
@@ -2437,7 +2440,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2477,7 +2480,7 @@
       <c r="M25">
         <v>5.5</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="5">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O25" t="s">
@@ -2499,7 +2502,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2539,7 +2542,7 @@
       <c r="M26">
         <v>5.6</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="5">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="O26" t="s">
@@ -2561,7 +2564,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2601,7 +2604,7 @@
       <c r="M27">
         <v>5.9</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="5">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="O27" t="s">
@@ -2623,7 +2626,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2663,7 +2666,7 @@
       <c r="M28">
         <v>6.6</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O28" t="s">
@@ -2685,7 +2688,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2725,7 +2728,7 @@
       <c r="M29">
         <v>6.5</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="5">
         <v>0.02</v>
       </c>
       <c r="O29" t="s">
@@ -2747,7 +2750,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2787,7 +2790,7 @@
       <c r="M30">
         <v>6.5</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="5">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="O30" t="s">
@@ -2809,7 +2812,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2849,7 +2852,7 @@
       <c r="M31">
         <v>5.6</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="5">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="O31" t="s">
@@ -2871,7 +2874,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2911,7 +2914,7 @@
       <c r="M32">
         <v>5.7</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="5">
         <v>1.9E-2</v>
       </c>
       <c r="O32" t="s">
@@ -2933,7 +2936,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2973,7 +2976,7 @@
       <c r="M33">
         <v>5.9</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="5">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O33" t="s">
@@ -2995,7 +2998,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3035,7 +3038,7 @@
       <c r="M34">
         <v>5.4</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="5">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="O34" t="s">
@@ -3057,7 +3060,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3097,7 +3100,7 @@
       <c r="M35">
         <v>5.6</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="5">
         <v>1.9E-2</v>
       </c>
       <c r="O35" t="s">
@@ -3119,7 +3122,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3159,7 +3162,7 @@
       <c r="M36">
         <v>6.1</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36" s="5">
         <v>0.02</v>
       </c>
       <c r="O36" t="s">
@@ -3181,7 +3184,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3221,7 +3224,7 @@
       <c r="M37">
         <v>6.6</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="5">
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="O37" t="s">
@@ -3243,7 +3246,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3283,7 +3286,7 @@
       <c r="M38">
         <v>6.8</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="O38" t="s">
@@ -3305,7 +3308,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3345,7 +3348,7 @@
       <c r="M39">
         <v>5.9</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="5">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="O39">
@@ -3367,7 +3370,7 @@
         <v>0.39300000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3407,7 +3410,7 @@
       <c r="M40">
         <v>5.9</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O40" t="s">
@@ -3429,7 +3432,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3469,7 +3472,7 @@
       <c r="M41">
         <v>5.9</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="5">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O41" t="s">
@@ -3491,7 +3494,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3531,7 +3534,7 @@
       <c r="M42" t="s">
         <v>107</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="N42" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O42" t="s">
@@ -3553,7 +3556,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3563,7 +3566,7 @@
       <c r="C43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="3">
         <v>3</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -3593,7 +3596,7 @@
       <c r="M43" s="2">
         <v>5.4</v>
       </c>
-      <c r="N43" s="2">
+      <c r="N43" s="5">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O43" s="2">
@@ -3615,7 +3618,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3625,7 +3628,7 @@
       <c r="C44" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="3">
         <v>2</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -3655,7 +3658,7 @@
       <c r="M44" s="2">
         <v>5.5500000000000007</v>
       </c>
-      <c r="N44" s="2">
+      <c r="N44" s="5">
         <v>2.8499999999999998E-2</v>
       </c>
       <c r="O44" s="2">
@@ -3677,7 +3680,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3687,7 +3690,7 @@
       <c r="C45" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="3">
         <v>3</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -3717,7 +3720,7 @@
       <c r="M45" s="2">
         <v>5.7</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="5">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="O45" s="2">
@@ -3739,7 +3742,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3749,7 +3752,7 @@
       <c r="C46" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="3">
         <v>1</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -3779,7 +3782,7 @@
       <c r="M46" s="2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="5">
         <v>9.5500000000000002E-2</v>
       </c>
       <c r="O46" s="2">
@@ -3801,7 +3804,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3811,7 +3814,7 @@
       <c r="C47" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="3">
         <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -3841,7 +3844,7 @@
       <c r="M47" s="2">
         <v>5.6</v>
       </c>
-      <c r="N47" s="2">
+      <c r="N47" s="5">
         <v>3.3500000000000002E-2</v>
       </c>
       <c r="O47" s="2">
@@ -3863,7 +3866,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3873,7 +3876,7 @@
       <c r="C48" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="3">
         <v>1</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -3903,7 +3906,7 @@
       <c r="M48" s="2">
         <v>5.15</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48" s="5">
         <v>0.10850000000000001</v>
       </c>
       <c r="O48" s="2">
@@ -3925,7 +3928,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3935,7 +3938,7 @@
       <c r="C49" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="3">
         <v>2</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -3965,7 +3968,7 @@
       <c r="M49" s="2">
         <v>5.65</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N49" s="5">
         <v>2.5499999999999998E-2</v>
       </c>
       <c r="O49" s="2">
@@ -3987,7 +3990,7 @@
         <v>65.25</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3997,7 +4000,7 @@
       <c r="C50" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="3">
         <v>3</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -4027,7 +4030,7 @@
       <c r="M50" s="2">
         <v>5.25</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="5">
         <v>2.3E-2</v>
       </c>
       <c r="O50" s="2">
@@ -4049,7 +4052,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -4059,7 +4062,7 @@
       <c r="C51" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="3">
         <v>1</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -4089,7 +4092,7 @@
       <c r="M51" s="2">
         <v>5.15</v>
       </c>
-      <c r="N51" s="2">
+      <c r="N51" s="5">
         <v>8.3500000000000005E-2</v>
       </c>
       <c r="O51" s="2">
@@ -4111,7 +4114,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -4121,7 +4124,7 @@
       <c r="C52" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="3">
         <v>2</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -4151,7 +4154,7 @@
       <c r="M52" s="2">
         <v>5.7</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N52" s="5">
         <v>2.7999999999999997E-2</v>
       </c>
       <c r="O52" s="2">
@@ -4173,7 +4176,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -4183,7 +4186,7 @@
       <c r="C53" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="3">
         <v>3</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -4213,7 +4216,7 @@
       <c r="M53" s="2">
         <v>5.4</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53" s="5">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O53" s="2">
@@ -4235,7 +4238,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -4245,7 +4248,7 @@
       <c r="C54" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>165</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -4275,7 +4278,7 @@
       <c r="M54" s="2">
         <v>5.25</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54" s="5">
         <v>8.8500000000000009E-2</v>
       </c>
       <c r="O54" s="2">
@@ -4297,7 +4300,7 @@
         <v>33.9465</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -4307,7 +4310,7 @@
       <c r="C55" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D55" s="3">
         <v>2</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -4337,7 +4340,7 @@
       <c r="M55" s="2">
         <v>5.25</v>
       </c>
-      <c r="N55" s="3">
+      <c r="N55" s="5">
         <v>2.75E-2</v>
       </c>
       <c r="O55" s="2">
@@ -4359,7 +4362,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4369,7 +4372,7 @@
       <c r="C56" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D56" s="3">
         <v>3</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -4399,7 +4402,7 @@
       <c r="M56" s="2">
         <v>5.45</v>
       </c>
-      <c r="N56" s="3">
+      <c r="N56" s="5">
         <v>2.35E-2</v>
       </c>
       <c r="O56" s="2">
@@ -4421,7 +4424,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4431,7 +4434,7 @@
       <c r="C57" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D57" s="3">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -4461,7 +4464,7 @@
       <c r="M57" s="2">
         <v>4.9499999999999993</v>
       </c>
-      <c r="N57" s="3">
+      <c r="N57" s="5">
         <v>9.0499999999999997E-2</v>
       </c>
       <c r="O57" s="2">
@@ -4483,7 +4486,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4493,7 +4496,7 @@
       <c r="C58" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="3">
         <v>2</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -4523,7 +4526,7 @@
       <c r="M58" s="2">
         <v>5.25</v>
       </c>
-      <c r="N58" s="3">
+      <c r="N58" s="5">
         <v>2.5499999999999998E-2</v>
       </c>
       <c r="O58" s="2">
@@ -4545,7 +4548,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4555,7 +4558,7 @@
       <c r="C59" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D59" s="3">
         <v>2</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -4585,7 +4588,7 @@
       <c r="M59" s="2">
         <v>5.7</v>
       </c>
-      <c r="N59" s="3">
+      <c r="N59" s="5">
         <v>2.4500000000000001E-2</v>
       </c>
       <c r="O59" s="2">
@@ -4607,7 +4610,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4617,7 +4620,7 @@
       <c r="C60" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D60" s="3">
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
@@ -4647,7 +4650,7 @@
       <c r="M60" s="2">
         <v>5.05</v>
       </c>
-      <c r="N60" s="3">
+      <c r="N60" s="5">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="O60" s="2">
@@ -4669,7 +4672,7 @@
         <v>60.6</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4679,7 +4682,7 @@
       <c r="C61" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D61" s="3">
         <v>2</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -4709,7 +4712,7 @@
       <c r="M61" s="2">
         <v>5.5</v>
       </c>
-      <c r="N61" s="3">
+      <c r="N61" s="5">
         <v>2.5499999999999998E-2</v>
       </c>
       <c r="O61" s="2">
@@ -4731,7 +4734,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4741,7 +4744,7 @@
       <c r="C62" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D62" s="3">
         <v>3</v>
       </c>
       <c r="E62" s="2" t="s">
@@ -4771,7 +4774,7 @@
       <c r="M62" s="2">
         <v>5.45</v>
       </c>
-      <c r="N62" s="3">
+      <c r="N62" s="5">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="O62" s="2">
@@ -4793,7 +4796,7 @@
         <v>75.5</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4803,7 +4806,7 @@
       <c r="C63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D63" s="3">
         <v>3</v>
       </c>
       <c r="E63" s="2" t="s">
@@ -4833,7 +4836,7 @@
       <c r="M63" s="2">
         <v>5.9</v>
       </c>
-      <c r="N63" s="2">
+      <c r="N63" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O63" s="2" t="s">
@@ -4855,7 +4858,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4865,7 +4868,7 @@
       <c r="C64" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D64" s="3">
         <v>2</v>
       </c>
       <c r="E64" s="2" t="s">
@@ -4895,7 +4898,7 @@
       <c r="M64" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N64" s="2" t="s">
+      <c r="N64" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O64" s="2" t="s">
@@ -4917,7 +4920,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4927,7 +4930,7 @@
       <c r="C65" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D65" s="3">
         <v>3</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -4957,7 +4960,7 @@
       <c r="M65" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N65" s="2" t="s">
+      <c r="N65" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O65" s="2" t="s">
@@ -4979,7 +4982,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4989,7 +4992,7 @@
       <c r="C66" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D66" s="3">
         <v>3</v>
       </c>
       <c r="E66" s="2" t="s">
@@ -5019,7 +5022,7 @@
       <c r="M66" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="N66" s="2">
+      <c r="N66" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O66" s="2" t="s">
@@ -5041,7 +5044,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -5051,7 +5054,7 @@
       <c r="C67" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D67" s="3">
         <v>1</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -5081,7 +5084,7 @@
       <c r="M67" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N67" s="2" t="s">
+      <c r="N67" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O67" s="2" t="s">
@@ -5103,7 +5106,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -5113,7 +5116,7 @@
       <c r="C68" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D68" s="3">
         <v>2</v>
       </c>
       <c r="E68" s="2" t="s">
@@ -5143,7 +5146,7 @@
       <c r="M68" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N68" s="2" t="s">
+      <c r="N68" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O68" s="2" t="s">
@@ -5165,7 +5168,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -5175,7 +5178,7 @@
       <c r="C69" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D69" s="3">
         <v>3</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -5205,7 +5208,7 @@
       <c r="M69" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N69" s="2" t="s">
+      <c r="N69" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O69" s="2" t="s">
@@ -5227,7 +5230,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -5237,7 +5240,7 @@
       <c r="C70" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D70" s="3">
         <v>3</v>
       </c>
       <c r="E70" s="2" t="s">
@@ -5267,7 +5270,7 @@
       <c r="M70" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N70" s="2" t="s">
+      <c r="N70" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O70" s="2" t="s">
@@ -5289,7 +5292,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -5299,7 +5302,7 @@
       <c r="C71" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D71" s="3">
         <v>2</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -5329,7 +5332,7 @@
       <c r="M71" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N71" s="2" t="s">
+      <c r="N71" s="5" t="s">
         <v>107</v>
       </c>
       <c r="O71" s="2" t="s">

</xml_diff>